<commit_message>
modified:   analisis_posicionamiento.ipynb 	modified:   salidas/analisis_posicionamiento.xlsx
</commit_message>
<xml_diff>
--- a/salidas/analisis_posicionamiento.xlsx
+++ b/salidas/analisis_posicionamiento.xlsx
@@ -8,9 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="sku_comp" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="familia_resumen" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="canal_vs_interno" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="precios_por_fuente" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="canal_vs_interno" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="precios_por_fuente" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20087,3110 +20086,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I99"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>familia</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>skus</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>precio_interno_prom</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>precio_externo_prom</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>gap_abs_prom</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>gap_abs_med</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>gap_pct_prom</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>gap_pct_med</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>gap_abs_total</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>ESPECIAS</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" t="n">
-        <v>11161.58212222467</v>
-      </c>
-      <c r="D2" t="n">
-        <v>21817.89350923856</v>
-      </c>
-      <c r="E2" t="n">
-        <v>10656.31138701389</v>
-      </c>
-      <c r="F2" t="n">
-        <v>3240.012605042018</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.7204854247191478</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.2905064068557973</v>
-      </c>
-      <c r="I2" t="n">
-        <v>10656.31138701389</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>ELABORADOS CRUDOS</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>5330</v>
-      </c>
-      <c r="D3" t="n">
-        <v>12324.9299719888</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6994.929971988797</v>
-      </c>
-      <c r="F3" t="n">
-        <v>6994.929971988797</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1.312369600748367</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.312369600748367</v>
-      </c>
-      <c r="I3" t="n">
-        <v>6994.929971988797</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>PORCIONADOS</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>13400</v>
-      </c>
-      <c r="D4" t="n">
-        <v>20059.63675792898</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6659.63675792898</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6659.63675792898</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.496987817755894</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.496987817755894</v>
-      </c>
-      <c r="I4" t="n">
-        <v>6659.63675792898</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>ACEITES VEGETALES</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2200</v>
-      </c>
-      <c r="D5" t="n">
-        <v>8486.55462184874</v>
-      </c>
-      <c r="E5" t="n">
-        <v>6286.55462184874</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6286.55462184874</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2.857524828113064</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2.857524828113064</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6286.55462184874</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>QUESOS DUROS</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>9900</v>
-      </c>
-      <c r="D6" t="n">
-        <v>15756.30252100841</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5856.302521008405</v>
-      </c>
-      <c r="F6" t="n">
-        <v>5856.302521008405</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.5915457091927683</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.5915457091927683</v>
-      </c>
-      <c r="I6" t="n">
-        <v>5856.302521008405</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>PLATOS PREPARADOS</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>8264.440990919649</v>
-      </c>
-      <c r="D7" t="n">
-        <v>12653.40534772668</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4388.964356807024</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5477.46371275783</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.5201870133848914</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.6342326404245908</v>
-      </c>
-      <c r="I7" t="n">
-        <v>4388.964356807026</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>SALSAS Y TOPPINGS</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>5514.705882352941</v>
-      </c>
-      <c r="D8" t="n">
-        <v>9873.949579831933</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4359.243697478992</v>
-      </c>
-      <c r="F8" t="n">
-        <v>4359.243697478992</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.7904761904761906</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.7904761904761906</v>
-      </c>
-      <c r="I8" t="n">
-        <v>4359.243697478992</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>CAFES DE GRANO ENTERO</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>25126</v>
-      </c>
-      <c r="D9" t="n">
-        <v>29117.64705882353</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3991.647058823532</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3991.647058823532</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.1588652017361909</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.1588652017361909</v>
-      </c>
-      <c r="I9" t="n">
-        <v>3991.647058823532</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>ACEITES DE OLIVA</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8550</v>
-      </c>
-      <c r="D10" t="n">
-        <v>12427.73109243697</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3877.731092436975</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3877.731092436975</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.4266194939514267</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.4266194939514267</v>
-      </c>
-      <c r="I10" t="n">
-        <v>3877.731092436974</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>MARISCOS Y MOLUSCOS</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-      <c r="C11" t="n">
-        <v>14395</v>
-      </c>
-      <c r="D11" t="n">
-        <v>18226.89075630252</v>
-      </c>
-      <c r="E11" t="n">
-        <v>3831.890756302521</v>
-      </c>
-      <c r="F11" t="n">
-        <v>3831.890756302521</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.2360351211724797</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.2360351211724797</v>
-      </c>
-      <c r="I11" t="n">
-        <v>3831.89075630252</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>MANTEQUILLA Y MARGARINA</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="n">
-        <v>5466.666666666667</v>
-      </c>
-      <c r="D12" t="n">
-        <v>9106.442577030813</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3639.775910364146</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2336.134453781513</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.1342036814725892</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.1342036814725892</v>
-      </c>
-      <c r="I12" t="n">
-        <v>3639.775910364147</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>OTROS APERITIVOS</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>12500</v>
-      </c>
-      <c r="D13" t="n">
-        <v>15957.98319327731</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3457.983193277312</v>
-      </c>
-      <c r="F13" t="n">
-        <v>3457.983193277312</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.2766386554621849</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.2766386554621849</v>
-      </c>
-      <c r="I13" t="n">
-        <v>3457.983193277312</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>SEMILLAS</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>5357.941834451902</v>
-      </c>
-      <c r="D14" t="n">
-        <v>8699.438324552619</v>
-      </c>
-      <c r="E14" t="n">
-        <v>3341.496490100717</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3341.496490100717</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.6236529983611776</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.6236529983611776</v>
-      </c>
-      <c r="I14" t="n">
-        <v>3341.496490100717</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>EMBUTIDOS Y FIAMBRES</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" t="n">
-        <v>9918.521457965902</v>
-      </c>
-      <c r="D15" t="n">
-        <v>13237.7656945131</v>
-      </c>
-      <c r="E15" t="n">
-        <v>3319.244236547198</v>
-      </c>
-      <c r="F15" t="n">
-        <v>3550.81684089758</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.3360744828231026</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.3665567863065868</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3319.244236547198</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>RELLENOS Y UNTABLES</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>11000</v>
-      </c>
-      <c r="D16" t="n">
-        <v>14281.71268507403</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3281.71268507403</v>
-      </c>
-      <c r="F16" t="n">
-        <v>3281.71268507403</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.2983375168249118</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.2983375168249118</v>
-      </c>
-      <c r="I16" t="n">
-        <v>3281.71268507403</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>CARNES VEGETALES</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="n">
-        <v>10789.47368421053</v>
-      </c>
-      <c r="D17" t="n">
-        <v>14064.57319770013</v>
-      </c>
-      <c r="E17" t="n">
-        <v>3275.099513489606</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3275.099513489606</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.3035458085673293</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.3035458085673293</v>
-      </c>
-      <c r="I17" t="n">
-        <v>3275.099513489606</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>EMPANADAS PARA FREIR</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="n">
-        <v>3025.793650793651</v>
-      </c>
-      <c r="D18" t="n">
-        <v>6231.2424969988</v>
-      </c>
-      <c r="E18" t="n">
-        <v>3205.448846205149</v>
-      </c>
-      <c r="F18" t="n">
-        <v>3205.448846205149</v>
-      </c>
-      <c r="G18" t="n">
-        <v>1.059374569499931</v>
-      </c>
-      <c r="H18" t="n">
-        <v>1.059374569499931</v>
-      </c>
-      <c r="I18" t="n">
-        <v>3205.448846205149</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>COBERTURAS Y DECORACIÃ“N</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" t="n">
-        <v>5388.235294117647</v>
-      </c>
-      <c r="D19" t="n">
-        <v>7626.505602240897</v>
-      </c>
-      <c r="E19" t="n">
-        <v>2238.270308123249</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2791.281512605042</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0.5090153777128568</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.7904761904761906</v>
-      </c>
-      <c r="I19" t="n">
-        <v>2238.27030812325</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>SALSAS ESPECIALES</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" t="n">
-        <v>3818.167892156863</v>
-      </c>
-      <c r="D20" t="n">
-        <v>5759.743022208883</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1941.575130052021</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1532.33793517407</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.4147759568935553</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.387515211689053</v>
-      </c>
-      <c r="I20" t="n">
-        <v>1941.575130052021</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>SYRUPS</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" t="n">
-        <v>12083.33333333333</v>
-      </c>
-      <c r="D21" t="n">
-        <v>13945.47152194211</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1862.138188608777</v>
-      </c>
-      <c r="F21" t="n">
-        <v>2471.288515406162</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.1541079880227954</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.2045204288611997</v>
-      </c>
-      <c r="I21" t="n">
-        <v>1862.138188608778</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>CAMARONES</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" t="n">
-        <v>7709.705882352941</v>
-      </c>
-      <c r="D22" t="n">
-        <v>9522.058823529413</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1812.352941176471</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1636.470588235295</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.2263705887974952</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.2159117859750517</v>
-      </c>
-      <c r="I22" t="n">
-        <v>1812.352941176472</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>TOCINOS</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>2</v>
-      </c>
-      <c r="C23" t="n">
-        <v>10063.32736798423</v>
-      </c>
-      <c r="D23" t="n">
-        <v>11818.6946366782</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1755.36726869397</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1755.36726869397</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.1813586885197848</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.1813586885197848</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1755.36726869397</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>CEREALES</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>8</v>
-      </c>
-      <c r="C24" t="n">
-        <v>5551.676242466684</v>
-      </c>
-      <c r="D24" t="n">
-        <v>7177.430241258715</v>
-      </c>
-      <c r="E24" t="n">
-        <v>1625.753998792031</v>
-      </c>
-      <c r="F24" t="n">
-        <v>2061.565126050421</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.2774971034052151</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.3165151635368243</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1625.753998792031</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>QUESOS</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" t="n">
-        <v>7826.666666666667</v>
-      </c>
-      <c r="D25" t="n">
-        <v>9446.978791516607</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1620.312124849941</v>
-      </c>
-      <c r="F25" t="n">
-        <v>152.8571428571431</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.1463921541354927</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.02186797465767421</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1620.31212484994</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>4</v>
-      </c>
-      <c r="C26" t="n">
-        <v>4554.166666666667</v>
-      </c>
-      <c r="D26" t="n">
-        <v>6045.745798319328</v>
-      </c>
-      <c r="E26" t="n">
-        <v>1491.579131652661</v>
-      </c>
-      <c r="F26" t="n">
-        <v>2325.210084033614</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.4494076140673804</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.6702778672444588</v>
-      </c>
-      <c r="I26" t="n">
-        <v>1491.579131652661</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>BOLLERIA PARA HORNEAR</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" t="n">
-        <v>4963.636363636364</v>
-      </c>
-      <c r="D27" t="n">
-        <v>6415.584415584416</v>
-      </c>
-      <c r="E27" t="n">
-        <v>1451.948051948052</v>
-      </c>
-      <c r="F27" t="n">
-        <v>1451.948051948052</v>
-      </c>
-      <c r="G27" t="n">
-        <v>0.2925170068027212</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.2925170068027212</v>
-      </c>
-      <c r="I27" t="n">
-        <v>1451.948051948052</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>Otros Abarrotes FS - Otros</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>2</v>
-      </c>
-      <c r="C28" t="n">
-        <v>2359.25</v>
-      </c>
-      <c r="D28" t="n">
-        <v>3649.84243697479</v>
-      </c>
-      <c r="E28" t="n">
-        <v>1290.59243697479</v>
-      </c>
-      <c r="F28" t="n">
-        <v>1290.59243697479</v>
-      </c>
-      <c r="G28" t="n">
-        <v>0.3125433246749664</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.3125433246749664</v>
-      </c>
-      <c r="I28" t="n">
-        <v>1290.59243697479</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>ENCURTIDOS</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>4</v>
-      </c>
-      <c r="C29" t="n">
-        <v>2865.242910061892</v>
-      </c>
-      <c r="D29" t="n">
-        <v>4140.93137254902</v>
-      </c>
-      <c r="E29" t="n">
-        <v>1275.688462487127</v>
-      </c>
-      <c r="F29" t="n">
-        <v>826.5998707175177</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0.3991597447415673</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0.3546482789582872</v>
-      </c>
-      <c r="I29" t="n">
-        <v>1275.688462487128</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>ELABORADOS</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" t="n">
-        <v>4916.666666666667</v>
-      </c>
-      <c r="D30" t="n">
-        <v>6049.019607843138</v>
-      </c>
-      <c r="E30" t="n">
-        <v>1132.352941176471</v>
-      </c>
-      <c r="F30" t="n">
-        <v>1132.352941176471</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0.2303090727816552</v>
-      </c>
-      <c r="H30" t="n">
-        <v>0.2303090727816552</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1132.352941176471</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>DESCONTINUADOS</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>9</v>
-      </c>
-      <c r="C31" t="n">
-        <v>6206.261742372854</v>
-      </c>
-      <c r="D31" t="n">
-        <v>7236.271445775137</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1030.009703402284</v>
-      </c>
-      <c r="F31" t="n">
-        <v>65.54621848739589</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0.120232104135476</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0.008193277310924563</v>
-      </c>
-      <c r="I31" t="n">
-        <v>1030.009703402283</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>PAPAS ESPECIALES</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>2400</v>
-      </c>
-      <c r="D32" t="n">
-        <v>3235.126050420168</v>
-      </c>
-      <c r="E32" t="n">
-        <v>835.1260504201682</v>
-      </c>
-      <c r="F32" t="n">
-        <v>835.1260504201682</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0.3479691876750701</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0.3479691876750701</v>
-      </c>
-      <c r="I32" t="n">
-        <v>835.1260504201682</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>MOSTAZAS</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1559.444444444444</v>
-      </c>
-      <c r="D33" t="n">
-        <v>2387.955182072829</v>
-      </c>
-      <c r="E33" t="n">
-        <v>828.5107376283848</v>
-      </c>
-      <c r="F33" t="n">
-        <v>828.5107376283848</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0.5839473944349065</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0.5839473944349065</v>
-      </c>
-      <c r="I33" t="n">
-        <v>828.510737628385</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>VERDURAS</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>13</v>
-      </c>
-      <c r="C34" t="n">
-        <v>2872.223409306743</v>
-      </c>
-      <c r="D34" t="n">
-        <v>3687.562011699267</v>
-      </c>
-      <c r="E34" t="n">
-        <v>815.3386023925242</v>
-      </c>
-      <c r="F34" t="n">
-        <v>130.4595912439054</v>
-      </c>
-      <c r="G34" t="n">
-        <v>0.1621026240972886</v>
-      </c>
-      <c r="H34" t="n">
-        <v>0.04064318034906278</v>
-      </c>
-      <c r="I34" t="n">
-        <v>815.3386023925241</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Pollo - Pollo</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D35" t="n">
-        <v>4774.509803921569</v>
-      </c>
-      <c r="E35" t="n">
-        <v>774.5098039215691</v>
-      </c>
-      <c r="F35" t="n">
-        <v>774.5098039215691</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0.1936274509803924</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0.1936274509803924</v>
-      </c>
-      <c r="I35" t="n">
-        <v>774.5098039215691</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>ACEITUNAS</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" t="n">
-        <v>5384.615384615385</v>
-      </c>
-      <c r="D36" t="n">
-        <v>6093.837535014006</v>
-      </c>
-      <c r="E36" t="n">
-        <v>709.2221503986211</v>
-      </c>
-      <c r="F36" t="n">
-        <v>709.2221503986211</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0.1317126850740296</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.1317126850740296</v>
-      </c>
-      <c r="I36" t="n">
-        <v>709.2221503986211</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>PAPAS FRITAS</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>5</v>
-      </c>
-      <c r="C37" t="n">
-        <v>10180.98857786358</v>
-      </c>
-      <c r="D37" t="n">
-        <v>10803.15222416063</v>
-      </c>
-      <c r="E37" t="n">
-        <v>622.1636462970504</v>
-      </c>
-      <c r="F37" t="n">
-        <v>926.7734423984439</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0.06710228982232269</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.07207228295217805</v>
-      </c>
-      <c r="I37" t="n">
-        <v>622.1636462970528</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>GALLETAS</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>16</v>
-      </c>
-      <c r="C38" t="n">
-        <v>5410.587571580024</v>
-      </c>
-      <c r="D38" t="n">
-        <v>6023.11451958257</v>
-      </c>
-      <c r="E38" t="n">
-        <v>612.5269480025456</v>
-      </c>
-      <c r="F38" t="n">
-        <v>421.3180981312717</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.09382170168434255</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.06574058449922771</v>
-      </c>
-      <c r="I38" t="n">
-        <v>612.5269480025463</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>BOLLERÃA LISTA PARA COMER</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>8</v>
-      </c>
-      <c r="C39" t="n">
-        <v>14682.98111542597</v>
-      </c>
-      <c r="D39" t="n">
-        <v>15249.86723001738</v>
-      </c>
-      <c r="E39" t="n">
-        <v>566.8861145914104</v>
-      </c>
-      <c r="F39" t="n">
-        <v>1262.379951980794</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0.09748198756202119</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0.1118274896165363</v>
-      </c>
-      <c r="I39" t="n">
-        <v>566.8861145914107</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>SALSAS DE SOYA</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" t="n">
-        <v>2957.671957671958</v>
-      </c>
-      <c r="D40" t="n">
-        <v>3514.578008981371</v>
-      </c>
-      <c r="E40" t="n">
-        <v>556.9060513094128</v>
-      </c>
-      <c r="F40" t="n">
-        <v>556.9060513094128</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0.1882920280813578</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0.1882920280813578</v>
-      </c>
-      <c r="I40" t="n">
-        <v>556.9060513094128</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>SALSAS DE AJI</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" t="n">
-        <v>1222.222222222222</v>
-      </c>
-      <c r="D41" t="n">
-        <v>1764.705882352941</v>
-      </c>
-      <c r="E41" t="n">
-        <v>542.483660130719</v>
-      </c>
-      <c r="F41" t="n">
-        <v>542.483660130719</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0.4438502673796791</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0.4438502673796791</v>
-      </c>
-      <c r="I41" t="n">
-        <v>542.483660130719</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>TORTILLAS DE MAIZ</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>2</v>
-      </c>
-      <c r="C42" t="n">
-        <v>3624.244812188075</v>
-      </c>
-      <c r="D42" t="n">
-        <v>4100.177107880188</v>
-      </c>
-      <c r="E42" t="n">
-        <v>475.9322956921142</v>
-      </c>
-      <c r="F42" t="n">
-        <v>475.9322956921142</v>
-      </c>
-      <c r="G42" t="n">
-        <v>0.1420585875479223</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0.1420585875479223</v>
-      </c>
-      <c r="I42" t="n">
-        <v>475.9322956921137</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>TORTILLAS DE TRIGO</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>2</v>
-      </c>
-      <c r="C43" t="n">
-        <v>3624.244812188075</v>
-      </c>
-      <c r="D43" t="n">
-        <v>4100.177107880188</v>
-      </c>
-      <c r="E43" t="n">
-        <v>475.9322956921142</v>
-      </c>
-      <c r="F43" t="n">
-        <v>475.9322956921142</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.1420585875479223</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0.1420585875479223</v>
-      </c>
-      <c r="I43" t="n">
-        <v>475.9322956921137</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>FRUTAS</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>4</v>
-      </c>
-      <c r="C44" t="n">
-        <v>5002.777777777777</v>
-      </c>
-      <c r="D44" t="n">
-        <v>5457.215389545649</v>
-      </c>
-      <c r="E44" t="n">
-        <v>454.4376117678712</v>
-      </c>
-      <c r="F44" t="n">
-        <v>330.403234740224</v>
-      </c>
-      <c r="G44" t="n">
-        <v>0.06970330223123214</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0.0413276471130038</v>
-      </c>
-      <c r="I44" t="n">
-        <v>454.4376117678712</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>SOPAS Y CREMAS</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>4</v>
-      </c>
-      <c r="C45" t="n">
-        <v>2031.975</v>
-      </c>
-      <c r="D45" t="n">
-        <v>2447.878151260504</v>
-      </c>
-      <c r="E45" t="n">
-        <v>415.9031512605043</v>
-      </c>
-      <c r="F45" t="n">
-        <v>506.05</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0.2116331224817848</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0.2380685583034194</v>
-      </c>
-      <c r="I45" t="n">
-        <v>415.9031512605043</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>CARNES PREMIUM</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>1</v>
-      </c>
-      <c r="C46" t="n">
-        <v>12590</v>
-      </c>
-      <c r="D46" t="n">
-        <v>12984.16666666667</v>
-      </c>
-      <c r="E46" t="n">
-        <v>394.1666666666661</v>
-      </c>
-      <c r="F46" t="n">
-        <v>394.1666666666661</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.03130791633571617</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.03130791633571617</v>
-      </c>
-      <c r="I46" t="n">
-        <v>394.1666666666661</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>JAMONES COCIDOS</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>2</v>
-      </c>
-      <c r="C47" t="n">
-        <v>9630</v>
-      </c>
-      <c r="D47" t="n">
-        <v>10019.04201680672</v>
-      </c>
-      <c r="E47" t="n">
-        <v>389.042016806723</v>
-      </c>
-      <c r="F47" t="n">
-        <v>389.042016806723</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.03012899758336474</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0.03012899758336474</v>
-      </c>
-      <c r="I47" t="n">
-        <v>389.042016806723</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>ACCESORIOS</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>1</v>
-      </c>
-      <c r="C48" t="n">
-        <v>8888.888888888889</v>
-      </c>
-      <c r="D48" t="n">
-        <v>9235.294117647059</v>
-      </c>
-      <c r="E48" t="n">
-        <v>346.4052287581708</v>
-      </c>
-      <c r="F48" t="n">
-        <v>346.4052287581708</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.0389705882352942</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.0389705882352942</v>
-      </c>
-      <c r="I48" t="n">
-        <v>346.4052287581708</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>VINAGRES</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>4</v>
-      </c>
-      <c r="C49" t="n">
-        <v>987.5</v>
-      </c>
-      <c r="D49" t="n">
-        <v>1315.441176470588</v>
-      </c>
-      <c r="E49" t="n">
-        <v>327.9411764705883</v>
-      </c>
-      <c r="F49" t="n">
-        <v>153.109243697479</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.2831698404645406</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0.1799530623060035</v>
-      </c>
-      <c r="I49" t="n">
-        <v>327.9411764705883</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>APANADOS</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>3</v>
-      </c>
-      <c r="C50" t="n">
-        <v>4850</v>
-      </c>
-      <c r="D50" t="n">
-        <v>5148.775910364147</v>
-      </c>
-      <c r="E50" t="n">
-        <v>298.7759103641462</v>
-      </c>
-      <c r="F50" t="n">
-        <v>774.5098039215691</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0.08151720334441419</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0.1936274509803924</v>
-      </c>
-      <c r="I50" t="n">
-        <v>298.7759103641465</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>MERMELADAS Y DULCES</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>4</v>
-      </c>
-      <c r="C51" t="n">
-        <v>6653.476190476191</v>
-      </c>
-      <c r="D51" t="n">
-        <v>6924.125010004002</v>
-      </c>
-      <c r="E51" t="n">
-        <v>270.6488195278114</v>
-      </c>
-      <c r="F51" t="n">
-        <v>-72.47899159663848</v>
-      </c>
-      <c r="G51" t="n">
-        <v>-0.01424085595802444</v>
-      </c>
-      <c r="H51" t="n">
-        <v>-0.02521008403361336</v>
-      </c>
-      <c r="I51" t="n">
-        <v>270.6488195278116</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>JUGOS</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>8</v>
-      </c>
-      <c r="C52" t="n">
-        <v>2630.527210884354</v>
-      </c>
-      <c r="D52" t="n">
-        <v>2874.834144183989</v>
-      </c>
-      <c r="E52" t="n">
-        <v>244.3069332996357</v>
-      </c>
-      <c r="F52" t="n">
-        <v>346.0318337861461</v>
-      </c>
-      <c r="G52" t="n">
-        <v>-0.03095750070363075</v>
-      </c>
-      <c r="H52" t="n">
-        <v>0.03284435688150855</v>
-      </c>
-      <c r="I52" t="n">
-        <v>244.3069332996356</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>PAPAS BASTON</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>2</v>
-      </c>
-      <c r="C53" t="n">
-        <v>2395</v>
-      </c>
-      <c r="D53" t="n">
-        <v>2637.352100840336</v>
-      </c>
-      <c r="E53" t="n">
-        <v>242.3521008403362</v>
-      </c>
-      <c r="F53" t="n">
-        <v>242.3521008403362</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0.114921901709872</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0.114921901709872</v>
-      </c>
-      <c r="I53" t="n">
-        <v>242.3521008403363</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>SUCEDANEOS DE LIMON</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" t="n">
-        <v>700</v>
-      </c>
-      <c r="D54" t="n">
-        <v>939.4957983193277</v>
-      </c>
-      <c r="E54" t="n">
-        <v>239.4957983193277</v>
-      </c>
-      <c r="F54" t="n">
-        <v>239.4957983193277</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0.3421368547418968</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0.3421368547418968</v>
-      </c>
-      <c r="I54" t="n">
-        <v>239.4957983193277</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>INGREDIENTES REPOSTERIA</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>8</v>
-      </c>
-      <c r="C55" t="n">
-        <v>5404.983853258413</v>
-      </c>
-      <c r="D55" t="n">
-        <v>5627.176710637753</v>
-      </c>
-      <c r="E55" t="n">
-        <v>222.1928573793405</v>
-      </c>
-      <c r="F55" t="n">
-        <v>-315.7563025210081</v>
-      </c>
-      <c r="G55" t="n">
-        <v>-0.05724029094150578</v>
-      </c>
-      <c r="H55" t="n">
-        <v>-0.1151754819574888</v>
-      </c>
-      <c r="I55" t="n">
-        <v>222.1928573793402</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>GUARNICIONES LISTAS</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>2</v>
-      </c>
-      <c r="C56" t="n">
-        <v>5577.777777777777</v>
-      </c>
-      <c r="D56" t="n">
-        <v>5716.526610644259</v>
-      </c>
-      <c r="E56" t="n">
-        <v>138.7488328664811</v>
-      </c>
-      <c r="F56" t="n">
-        <v>138.7488328664811</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0.09933830271518113</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0.09933830271518113</v>
-      </c>
-      <c r="I56" t="n">
-        <v>138.7488328664813</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>PASTAS</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>14</v>
-      </c>
-      <c r="C57" t="n">
-        <v>2080.327248677248</v>
-      </c>
-      <c r="D57" t="n">
-        <v>2216.34017243261</v>
-      </c>
-      <c r="E57" t="n">
-        <v>136.0129237553608</v>
-      </c>
-      <c r="F57" t="n">
-        <v>55.13277310924389</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0.04691991091856773</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0.03101997093189379</v>
-      </c>
-      <c r="I57" t="n">
-        <v>136.012923755361</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>SALSAS DE TOMATE</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>4</v>
-      </c>
-      <c r="C58" t="n">
-        <v>2949.007936507936</v>
-      </c>
-      <c r="D58" t="n">
-        <v>3071.424719887956</v>
-      </c>
-      <c r="E58" t="n">
-        <v>122.4167833800191</v>
-      </c>
-      <c r="F58" t="n">
-        <v>-0.04668534080292375</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0.01813954682055169</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0.01839122652671177</v>
-      </c>
-      <c r="I58" t="n">
-        <v>122.4167833800193</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>AGUAS</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>2</v>
-      </c>
-      <c r="C59" t="n">
-        <v>1530.30303030303</v>
-      </c>
-      <c r="D59" t="n">
-        <v>1610.351678550208</v>
-      </c>
-      <c r="E59" t="n">
-        <v>80.04864824717754</v>
-      </c>
-      <c r="F59" t="n">
-        <v>80.04864824717754</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0.09181862745098035</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0.09181862745098035</v>
-      </c>
-      <c r="I59" t="n">
-        <v>80.04864824717743</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>POSTRES EN POLVO</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>6</v>
-      </c>
-      <c r="C60" t="n">
-        <v>4038.75</v>
-      </c>
-      <c r="D60" t="n">
-        <v>4107.03781512605</v>
-      </c>
-      <c r="E60" t="n">
-        <v>68.28781512605048</v>
-      </c>
-      <c r="F60" t="n">
-        <v>-540.7563025210084</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0.04196736896201066</v>
-      </c>
-      <c r="H60" t="n">
-        <v>-0.1162916779615072</v>
-      </c>
-      <c r="I60" t="n">
-        <v>68.28781512605019</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>CALDOS Y BASES</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>1</v>
-      </c>
-      <c r="C61" t="n">
-        <v>1950</v>
-      </c>
-      <c r="D61" t="n">
-        <v>2008.403361344538</v>
-      </c>
-      <c r="E61" t="n">
-        <v>58.40336134453787</v>
-      </c>
-      <c r="F61" t="n">
-        <v>58.40336134453787</v>
-      </c>
-      <c r="G61" t="n">
-        <v>0.02995044171514771</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0.02995044171514771</v>
-      </c>
-      <c r="I61" t="n">
-        <v>58.40336134453787</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>KETCHUP</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>2</v>
-      </c>
-      <c r="C62" t="n">
-        <v>2358.333333333333</v>
-      </c>
-      <c r="D62" t="n">
-        <v>2404.295051353875</v>
-      </c>
-      <c r="E62" t="n">
-        <v>45.96171802054164</v>
-      </c>
-      <c r="F62" t="n">
-        <v>45.96171802054164</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0.02175181872124787</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0.02175181872124787</v>
-      </c>
-      <c r="I62" t="n">
-        <v>45.96171802054141</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>MEZCLAS ESPECIALES</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>2</v>
-      </c>
-      <c r="C63" t="n">
-        <v>2025</v>
-      </c>
-      <c r="D63" t="n">
-        <v>2056.063025210084</v>
-      </c>
-      <c r="E63" t="n">
-        <v>31.06302521008411</v>
-      </c>
-      <c r="F63" t="n">
-        <v>31.06302521008411</v>
-      </c>
-      <c r="G63" t="n">
-        <v>0.01646443943431036</v>
-      </c>
-      <c r="H63" t="n">
-        <v>0.01646443943431036</v>
-      </c>
-      <c r="I63" t="n">
-        <v>31.06302521008411</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>QUESOS SEMI DUROS</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>3</v>
-      </c>
-      <c r="C64" t="n">
-        <v>6923.421828908555</v>
-      </c>
-      <c r="D64" t="n">
-        <v>6939.975990396159</v>
-      </c>
-      <c r="E64" t="n">
-        <v>16.55416148760469</v>
-      </c>
-      <c r="F64" t="n">
-        <v>152.8571428571431</v>
-      </c>
-      <c r="G64" t="n">
-        <v>-0.002343293423484309</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0.02186797465767421</v>
-      </c>
-      <c r="I64" t="n">
-        <v>16.55416148760469</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>MAYONESAS</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>4</v>
-      </c>
-      <c r="C65" t="n">
-        <v>2895.47514619883</v>
-      </c>
-      <c r="D65" t="n">
-        <v>2854.190159740872</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-41.28498645795798</v>
-      </c>
-      <c r="F65" t="n">
-        <v>59.21832134915849</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0.1006706680371804</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0.0209699832892149</v>
-      </c>
-      <c r="I65" t="n">
-        <v>-41.28498645795798</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>SAL</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>1</v>
-      </c>
-      <c r="C66" t="n">
-        <v>411.8</v>
-      </c>
-      <c r="D66" t="n">
-        <v>365.1974789915967</v>
-      </c>
-      <c r="E66" t="n">
-        <v>-46.60252100840336</v>
-      </c>
-      <c r="F66" t="n">
-        <v>-46.60252100840336</v>
-      </c>
-      <c r="G66" t="n">
-        <v>-0.1131678509189008</v>
-      </c>
-      <c r="H66" t="n">
-        <v>-0.1131678509189008</v>
-      </c>
-      <c r="I66" t="n">
-        <v>-46.60252100840336</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>Arroz</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>1</v>
-      </c>
-      <c r="C67" t="n">
-        <v>2500</v>
-      </c>
-      <c r="D67" t="n">
-        <v>2435.294117647059</v>
-      </c>
-      <c r="E67" t="n">
-        <v>-64.70588235294099</v>
-      </c>
-      <c r="F67" t="n">
-        <v>-64.70588235294099</v>
-      </c>
-      <c r="G67" t="n">
-        <v>-0.02588235294117636</v>
-      </c>
-      <c r="H67" t="n">
-        <v>-0.02588235294117636</v>
-      </c>
-      <c r="I67" t="n">
-        <v>-64.70588235294099</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>FILETILLOS</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>1</v>
-      </c>
-      <c r="C68" t="n">
-        <v>5800</v>
-      </c>
-      <c r="D68" t="n">
-        <v>5670</v>
-      </c>
-      <c r="E68" t="n">
-        <v>-130</v>
-      </c>
-      <c r="F68" t="n">
-        <v>-130</v>
-      </c>
-      <c r="G68" t="n">
-        <v>-0.02241379310344827</v>
-      </c>
-      <c r="H68" t="n">
-        <v>-0.02241379310344827</v>
-      </c>
-      <c r="I68" t="n">
-        <v>-130</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>GRASAS CULINARIAS</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>2</v>
-      </c>
-      <c r="C69" t="n">
-        <v>4890.532926147361</v>
-      </c>
-      <c r="D69" t="n">
-        <v>4756.302521008403</v>
-      </c>
-      <c r="E69" t="n">
-        <v>-134.2304051389569</v>
-      </c>
-      <c r="F69" t="n">
-        <v>-134.2304051389569</v>
-      </c>
-      <c r="G69" t="n">
-        <v>-0.03685203873158027</v>
-      </c>
-      <c r="H69" t="n">
-        <v>-0.03685203873158027</v>
-      </c>
-      <c r="I69" t="n">
-        <v>-134.2304051389574</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>ARROZ</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>6</v>
-      </c>
-      <c r="C70" t="n">
-        <v>1947.833333333333</v>
-      </c>
-      <c r="D70" t="n">
-        <v>1776.659663865546</v>
-      </c>
-      <c r="E70" t="n">
-        <v>-171.1736694677871</v>
-      </c>
-      <c r="F70" t="n">
-        <v>-494.7924369747899</v>
-      </c>
-      <c r="G70" t="n">
-        <v>-0.09531825936017695</v>
-      </c>
-      <c r="H70" t="n">
-        <v>-0.224415407864375</v>
-      </c>
-      <c r="I70" t="n">
-        <v>-171.1736694677868</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>YOGHURT</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>9</v>
-      </c>
-      <c r="C71" t="n">
-        <v>1736.32809577254</v>
-      </c>
-      <c r="D71" t="n">
-        <v>1559.070442992012</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-177.2576527805286</v>
-      </c>
-      <c r="F71" t="n">
-        <v>-310.9943977591035</v>
-      </c>
-      <c r="G71" t="n">
-        <v>-0.1057619049575629</v>
-      </c>
-      <c r="H71" t="n">
-        <v>-0.1561478147744453</v>
-      </c>
-      <c r="I71" t="n">
-        <v>-177.2576527805288</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>HARINAS Y SEMOLAS</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>3</v>
-      </c>
-      <c r="C72" t="n">
-        <v>1640.833333333333</v>
-      </c>
-      <c r="D72" t="n">
-        <v>1442.201680672269</v>
-      </c>
-      <c r="E72" t="n">
-        <v>-198.6316526610643</v>
-      </c>
-      <c r="F72" t="n">
-        <v>-140.3249299719887</v>
-      </c>
-      <c r="G72" t="n">
-        <v>-0.1788158526138066</v>
-      </c>
-      <c r="H72" t="n">
-        <v>-0.1322068998539587</v>
-      </c>
-      <c r="I72" t="n">
-        <v>-198.6316526610642</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>AZUCAR Y ENDULZANTES</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" t="n">
-        <v>1218.5</v>
-      </c>
-      <c r="D73" t="n">
-        <v>1008.403361344538</v>
-      </c>
-      <c r="E73" t="n">
-        <v>-210.0966386554621</v>
-      </c>
-      <c r="F73" t="n">
-        <v>-210.0966386554621</v>
-      </c>
-      <c r="G73" t="n">
-        <v>-0.1724223542515076</v>
-      </c>
-      <c r="H73" t="n">
-        <v>-0.1724223542515076</v>
-      </c>
-      <c r="I73" t="n">
-        <v>-210.0966386554621</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>OTROS SNACKS</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>1</v>
-      </c>
-      <c r="C74" t="n">
-        <v>5806.899441252001</v>
-      </c>
-      <c r="D74" t="n">
-        <v>5587.778589696749</v>
-      </c>
-      <c r="E74" t="n">
-        <v>-219.1208515552516</v>
-      </c>
-      <c r="F74" t="n">
-        <v>-219.1208515552516</v>
-      </c>
-      <c r="G74" t="n">
-        <v>-0.03773456967389954</v>
-      </c>
-      <c r="H74" t="n">
-        <v>-0.03773456967389954</v>
-      </c>
-      <c r="I74" t="n">
-        <v>-219.1208515552516</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>IsotÃ³nica y EnergÃ©tica</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>2</v>
-      </c>
-      <c r="C75" t="n">
-        <v>1633.928571428572</v>
-      </c>
-      <c r="D75" t="n">
-        <v>1389.64409293129</v>
-      </c>
-      <c r="E75" t="n">
-        <v>-244.2844784972814</v>
-      </c>
-      <c r="F75" t="n">
-        <v>-244.2844784972814</v>
-      </c>
-      <c r="G75" t="n">
-        <v>-0.1495074403917788</v>
-      </c>
-      <c r="H75" t="n">
-        <v>-0.1495074403917788</v>
-      </c>
-      <c r="I75" t="n">
-        <v>-244.2844784972813</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>ELABORADOS COCIDOS</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C76" t="n">
-        <v>5980</v>
-      </c>
-      <c r="D76" t="n">
-        <v>5697.5</v>
-      </c>
-      <c r="E76" t="n">
-        <v>-282.5</v>
-      </c>
-      <c r="F76" t="n">
-        <v>-282.5</v>
-      </c>
-      <c r="G76" t="n">
-        <v>-0.04724080267558528</v>
-      </c>
-      <c r="H76" t="n">
-        <v>-0.04724080267558528</v>
-      </c>
-      <c r="I76" t="n">
-        <v>-282.5</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>PANES LISTOS PARA COMER</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>1</v>
-      </c>
-      <c r="C77" t="n">
-        <v>3748.326639892905</v>
-      </c>
-      <c r="D77" t="n">
-        <v>3450.571428571428</v>
-      </c>
-      <c r="E77" t="n">
-        <v>-297.7552113214765</v>
-      </c>
-      <c r="F77" t="n">
-        <v>-297.7552113214765</v>
-      </c>
-      <c r="G77" t="n">
-        <v>-0.07943683673469393</v>
-      </c>
-      <c r="H77" t="n">
-        <v>-0.07943683673469393</v>
-      </c>
-      <c r="I77" t="n">
-        <v>-297.7552113214765</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>PANES PARA HORNEAR</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C78" t="n">
-        <v>3748.326639892905</v>
-      </c>
-      <c r="D78" t="n">
-        <v>3450.571428571428</v>
-      </c>
-      <c r="E78" t="n">
-        <v>-297.7552113214765</v>
-      </c>
-      <c r="F78" t="n">
-        <v>-297.7552113214765</v>
-      </c>
-      <c r="G78" t="n">
-        <v>-0.07943683673469393</v>
-      </c>
-      <c r="H78" t="n">
-        <v>-0.07943683673469393</v>
-      </c>
-      <c r="I78" t="n">
-        <v>-297.7552113214765</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>LEGUMBRES</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>4</v>
-      </c>
-      <c r="C79" t="n">
-        <v>2540</v>
-      </c>
-      <c r="D79" t="n">
-        <v>2148.949579831933</v>
-      </c>
-      <c r="E79" t="n">
-        <v>-391.0504201680673</v>
-      </c>
-      <c r="F79" t="n">
-        <v>-350</v>
-      </c>
-      <c r="G79" t="n">
-        <v>-0.1531616668280907</v>
-      </c>
-      <c r="H79" t="n">
-        <v>-0.1378388345933985</v>
-      </c>
-      <c r="I79" t="n">
-        <v>-391.0504201680674</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>LECHES</t>
-        </is>
-      </c>
-      <c r="B80" t="n">
-        <v>5</v>
-      </c>
-      <c r="C80" t="n">
-        <v>2705.861111111111</v>
-      </c>
-      <c r="D80" t="n">
-        <v>2313.108590102708</v>
-      </c>
-      <c r="E80" t="n">
-        <v>-392.7525210084033</v>
-      </c>
-      <c r="F80" t="n">
-        <v>-308.6330532212885</v>
-      </c>
-      <c r="G80" t="n">
-        <v>-0.1455259358891337</v>
-      </c>
-      <c r="H80" t="n">
-        <v>-0.1480724297671354</v>
-      </c>
-      <c r="I80" t="n">
-        <v>-392.7525210084032</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>BEBIDAS GASEOSAS</t>
-        </is>
-      </c>
-      <c r="B81" t="n">
-        <v>2</v>
-      </c>
-      <c r="C81" t="n">
-        <v>2107.142857142857</v>
-      </c>
-      <c r="D81" t="n">
-        <v>1696.678671468588</v>
-      </c>
-      <c r="E81" t="n">
-        <v>-410.4641856742695</v>
-      </c>
-      <c r="F81" t="n">
-        <v>-410.4641856742695</v>
-      </c>
-      <c r="G81" t="n">
-        <v>-0.1878448349036583</v>
-      </c>
-      <c r="H81" t="n">
-        <v>-0.1878448349036583</v>
-      </c>
-      <c r="I81" t="n">
-        <v>-410.4641856742692</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>QUESOS BLANDOS</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>4</v>
-      </c>
-      <c r="C82" t="n">
-        <v>11691.76470588235</v>
-      </c>
-      <c r="D82" t="n">
-        <v>11234.07377656945</v>
-      </c>
-      <c r="E82" t="n">
-        <v>-457.690929312902</v>
-      </c>
-      <c r="F82" t="n">
-        <v>-1553.293376173999</v>
-      </c>
-      <c r="G82" t="n">
-        <v>-0.01300172876542233</v>
-      </c>
-      <c r="H82" t="n">
-        <v>-0.123969786919743</v>
-      </c>
-      <c r="I82" t="n">
-        <v>-457.6909293129029</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>TE Y OTRAS BEBIDAS CALIENTES</t>
-        </is>
-      </c>
-      <c r="B83" t="n">
-        <v>6</v>
-      </c>
-      <c r="C83" t="n">
-        <v>38858.79737546405</v>
-      </c>
-      <c r="D83" t="n">
-        <v>38320.10582010582</v>
-      </c>
-      <c r="E83" t="n">
-        <v>-538.6915553582212</v>
-      </c>
-      <c r="F83" t="n">
-        <v>-2455.648926237158</v>
-      </c>
-      <c r="G83" t="n">
-        <v>-0.0597207743312379</v>
-      </c>
-      <c r="H83" t="n">
-        <v>-0.1034913965586234</v>
-      </c>
-      <c r="I83" t="n">
-        <v>-538.6915553582294</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>ACETOS BALSAMICOS</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>1</v>
-      </c>
-      <c r="C84" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D84" t="n">
-        <v>5121.8</v>
-      </c>
-      <c r="E84" t="n">
-        <v>-878.1999999999998</v>
-      </c>
-      <c r="F84" t="n">
-        <v>-878.1999999999998</v>
-      </c>
-      <c r="G84" t="n">
-        <v>-0.1463666666666666</v>
-      </c>
-      <c r="H84" t="n">
-        <v>-0.1463666666666666</v>
-      </c>
-      <c r="I84" t="n">
-        <v>-878.1999999999998</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>APERITIVOS ORIENTALES</t>
-        </is>
-      </c>
-      <c r="B85" t="n">
-        <v>4</v>
-      </c>
-      <c r="C85" t="n">
-        <v>7564.910714285714</v>
-      </c>
-      <c r="D85" t="n">
-        <v>6668.435707616381</v>
-      </c>
-      <c r="E85" t="n">
-        <v>-896.4750066693338</v>
-      </c>
-      <c r="F85" t="n">
-        <v>-1319.779078297986</v>
-      </c>
-      <c r="G85" t="n">
-        <v>-0.1526389834538529</v>
-      </c>
-      <c r="H85" t="n">
-        <v>-0.1926334866161667</v>
-      </c>
-      <c r="I85" t="n">
-        <v>-896.4750066693332</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>PESCADOS</t>
-        </is>
-      </c>
-      <c r="B86" t="n">
-        <v>2</v>
-      </c>
-      <c r="C86" t="n">
-        <v>15835</v>
-      </c>
-      <c r="D86" t="n">
-        <v>14823.52941176471</v>
-      </c>
-      <c r="E86" t="n">
-        <v>-1011.470588235294</v>
-      </c>
-      <c r="F86" t="n">
-        <v>-1011.470588235294</v>
-      </c>
-      <c r="G86" t="n">
-        <v>0.04143722224159174</v>
-      </c>
-      <c r="H86" t="n">
-        <v>0.04143722224159174</v>
-      </c>
-      <c r="I86" t="n">
-        <v>-1011.470588235294</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>PECHUGAS</t>
-        </is>
-      </c>
-      <c r="B87" t="n">
-        <v>2</v>
-      </c>
-      <c r="C87" t="n">
-        <v>7083.333333333333</v>
-      </c>
-      <c r="D87" t="n">
-        <v>5986.194477791117</v>
-      </c>
-      <c r="E87" t="n">
-        <v>-1097.138855542216</v>
-      </c>
-      <c r="F87" t="n">
-        <v>-1097.138855542216</v>
-      </c>
-      <c r="G87" t="n">
-        <v>-0.1358435117418309</v>
-      </c>
-      <c r="H87" t="n">
-        <v>-0.1358435117418309</v>
-      </c>
-      <c r="I87" t="n">
-        <v>-1097.138855542216</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>JUGOS Y PULPAS</t>
-        </is>
-      </c>
-      <c r="B88" t="n">
-        <v>1</v>
-      </c>
-      <c r="C88" t="n">
-        <v>6600</v>
-      </c>
-      <c r="D88" t="n">
-        <v>5497</v>
-      </c>
-      <c r="E88" t="n">
-        <v>-1103</v>
-      </c>
-      <c r="F88" t="n">
-        <v>-1103</v>
-      </c>
-      <c r="G88" t="n">
-        <v>-0.1671212121212121</v>
-      </c>
-      <c r="H88" t="n">
-        <v>-0.1671212121212121</v>
-      </c>
-      <c r="I88" t="n">
-        <v>-1103</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="1" t="inlineStr">
-        <is>
-          <t>TRUTROS</t>
-        </is>
-      </c>
-      <c r="B89" t="n">
-        <v>1</v>
-      </c>
-      <c r="C89" t="n">
-        <v>3300</v>
-      </c>
-      <c r="D89" t="n">
-        <v>2190</v>
-      </c>
-      <c r="E89" t="n">
-        <v>-1110</v>
-      </c>
-      <c r="F89" t="n">
-        <v>-1110</v>
-      </c>
-      <c r="G89" t="n">
-        <v>-0.3363636363636363</v>
-      </c>
-      <c r="H89" t="n">
-        <v>-0.3363636363636363</v>
-      </c>
-      <c r="I89" t="n">
-        <v>-1110</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>FRUTOS SECOS</t>
-        </is>
-      </c>
-      <c r="B90" t="n">
-        <v>6</v>
-      </c>
-      <c r="C90" t="n">
-        <v>8948.333333333334</v>
-      </c>
-      <c r="D90" t="n">
-        <v>7423.878151260505</v>
-      </c>
-      <c r="E90" t="n">
-        <v>-1524.455182072829</v>
-      </c>
-      <c r="F90" t="n">
-        <v>-478.1932773109238</v>
-      </c>
-      <c r="G90" t="n">
-        <v>-0.1401751749656572</v>
-      </c>
-      <c r="H90" t="n">
-        <v>-0.05981413216099951</v>
-      </c>
-      <c r="I90" t="n">
-        <v>-1524.455182072829</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="1" t="inlineStr">
-        <is>
-          <t>SALMONES</t>
-        </is>
-      </c>
-      <c r="B91" t="n">
-        <v>3</v>
-      </c>
-      <c r="C91" t="n">
-        <v>14190</v>
-      </c>
-      <c r="D91" t="n">
-        <v>12575.02801120448</v>
-      </c>
-      <c r="E91" t="n">
-        <v>-1614.971988795518</v>
-      </c>
-      <c r="F91" t="n">
-        <v>225</v>
-      </c>
-      <c r="G91" t="n">
-        <v>-0.06626993906629368</v>
-      </c>
-      <c r="H91" t="n">
-        <v>0.02499999999999991</v>
-      </c>
-      <c r="I91" t="n">
-        <v>-1614.97198879552</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>PESCADOS EN CONSERVA</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
-        <v>1</v>
-      </c>
-      <c r="C92" t="n">
-        <v>7941.176470588236</v>
-      </c>
-      <c r="D92" t="n">
-        <v>6223.73949579832</v>
-      </c>
-      <c r="E92" t="n">
-        <v>-1717.436974789916</v>
-      </c>
-      <c r="F92" t="n">
-        <v>-1717.436974789916</v>
-      </c>
-      <c r="G92" t="n">
-        <v>-0.2162698412698413</v>
-      </c>
-      <c r="H92" t="n">
-        <v>-0.2162698412698413</v>
-      </c>
-      <c r="I92" t="n">
-        <v>-1717.436974789916</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="1" t="inlineStr">
-        <is>
-          <t>CARNES CERTIFICADAS</t>
-        </is>
-      </c>
-      <c r="B93" t="n">
-        <v>2</v>
-      </c>
-      <c r="C93" t="n">
-        <v>33250</v>
-      </c>
-      <c r="D93" t="n">
-        <v>31084.03361344538</v>
-      </c>
-      <c r="E93" t="n">
-        <v>-2165.966386554621</v>
-      </c>
-      <c r="F93" t="n">
-        <v>-2165.966386554621</v>
-      </c>
-      <c r="G93" t="n">
-        <v>-0.06084132880776116</v>
-      </c>
-      <c r="H93" t="n">
-        <v>-0.06084132880776116</v>
-      </c>
-      <c r="I93" t="n">
-        <v>-2165.966386554621</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>HELADOS</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>2</v>
-      </c>
-      <c r="C94" t="n">
-        <v>5576.670692431561</v>
-      </c>
-      <c r="D94" t="n">
-        <v>2387.629260037349</v>
-      </c>
-      <c r="E94" t="n">
-        <v>-3189.041432394213</v>
-      </c>
-      <c r="F94" t="n">
-        <v>-4077.497665732959</v>
-      </c>
-      <c r="G94" t="n">
-        <v>-0.5492393111245221</v>
-      </c>
-      <c r="H94" t="n">
-        <v>-0.6672268907563025</v>
-      </c>
-      <c r="I94" t="n">
-        <v>-3189.041432394213</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="1" t="inlineStr">
-        <is>
-          <t>DULCES Y CHOCOLATES</t>
-        </is>
-      </c>
-      <c r="B95" t="n">
-        <v>4</v>
-      </c>
-      <c r="C95" t="n">
-        <v>31307.39096429886</v>
-      </c>
-      <c r="D95" t="n">
-        <v>27073.62898539369</v>
-      </c>
-      <c r="E95" t="n">
-        <v>-4233.761978905167</v>
-      </c>
-      <c r="F95" t="n">
-        <v>-3918.25821237586</v>
-      </c>
-      <c r="G95" t="n">
-        <v>-0.046234770867044</v>
-      </c>
-      <c r="H95" t="n">
-        <v>-0.079185520361991</v>
-      </c>
-      <c r="I95" t="n">
-        <v>-4233.761978905168</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="1" t="inlineStr">
-        <is>
-          <t>Chocolates - Rocher - Rocher</t>
-        </is>
-      </c>
-      <c r="B96" t="n">
-        <v>1</v>
-      </c>
-      <c r="C96" t="n">
-        <v>52000</v>
-      </c>
-      <c r="D96" t="n">
-        <v>44201.68067226891</v>
-      </c>
-      <c r="E96" t="n">
-        <v>-7798.319327731093</v>
-      </c>
-      <c r="F96" t="n">
-        <v>-7798.319327731093</v>
-      </c>
-      <c r="G96" t="n">
-        <v>-0.1499676793794441</v>
-      </c>
-      <c r="H96" t="n">
-        <v>-0.1499676793794441</v>
-      </c>
-      <c r="I96" t="n">
-        <v>-7798.319327731093</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="1" t="inlineStr">
-        <is>
-          <t>CAFES SOLUBLES</t>
-        </is>
-      </c>
-      <c r="B97" t="n">
-        <v>3</v>
-      </c>
-      <c r="C97" t="n">
-        <v>50087.11913884329</v>
-      </c>
-      <c r="D97" t="n">
-        <v>39594.23980341607</v>
-      </c>
-      <c r="E97" t="n">
-        <v>-10492.87933542721</v>
-      </c>
-      <c r="F97" t="n">
-        <v>-14762.5716953448</v>
-      </c>
-      <c r="G97" t="n">
-        <v>-0.1571241855693292</v>
-      </c>
-      <c r="H97" t="n">
-        <v>-0.222680510719632</v>
-      </c>
-      <c r="I97" t="n">
-        <v>-10492.87933542721</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>Ferrero - Ferrero</t>
-        </is>
-      </c>
-      <c r="B98" t="n">
-        <v>1</v>
-      </c>
-      <c r="C98" t="n">
-        <v>42105.26315789474</v>
-      </c>
-      <c r="D98" t="n">
-        <v>19346.40522875817</v>
-      </c>
-      <c r="E98" t="n">
-        <v>-22758.85792913657</v>
-      </c>
-      <c r="F98" t="n">
-        <v>-22758.85792913657</v>
-      </c>
-      <c r="G98" t="n">
-        <v>-0.5405228758169934</v>
-      </c>
-      <c r="H98" t="n">
-        <v>-0.5405228758169934</v>
-      </c>
-      <c r="I98" t="n">
-        <v>-22758.85792913657</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="1" t="inlineStr">
-        <is>
-          <t>MINI PORCIONES</t>
-        </is>
-      </c>
-      <c r="B99" t="n">
-        <v>17</v>
-      </c>
-      <c r="C99" t="n">
-        <v>169108.8368983957</v>
-      </c>
-      <c r="D99" t="n">
-        <v>8748.013010432931</v>
-      </c>
-      <c r="E99" t="n">
-        <v>-160360.8238879628</v>
-      </c>
-      <c r="F99" t="n">
-        <v>803.5714285714284</v>
-      </c>
-      <c r="G99" t="n">
-        <v>0.2143918851437825</v>
-      </c>
-      <c r="H99" t="n">
-        <v>0.2331941176470587</v>
-      </c>
-      <c r="I99" t="n">
-        <v>-160360.8238879628</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23271,7 +20166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>